<commit_message>
updated calculations, new offseting choices structure with planetary boundaries as the largest group, start of a white paper explaining the calculations
</commit_message>
<xml_diff>
--- a/calculations/animal_walfare/animal_walfare.xlsx
+++ b/calculations/animal_walfare/animal_walfare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sucha\programming\offset_me\calculations\animal_walfare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32618DEC-7FB2-4B19-8BA1-6A4302800C12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1898705-8EF1-4279-9D2A-535792BD8142}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6975" yWindow="2655" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Farm animals" sheetId="1" r:id="rId1"/>

</xml_diff>